<commit_message>
better water color map
</commit_message>
<xml_diff>
--- a/final_geo_data/csv/obvious_poi.xlsx
+++ b/final_geo_data/csv/obvious_poi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rainylty/STUDY/IVth/datascience/summer_school/summoning_and_lotr/Viz_of_Summoning_and_Middle_Earth/final_geo_data/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D132B04-3C87-CF4E-8CBE-6D277B2753D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0949E6B6-9A47-504C-86D6-BDD0BF0731A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5540" yWindow="500" windowWidth="28980" windowHeight="21900" xr2:uid="{81031926-05D2-A343-B9B8-A8769874A27F}"/>
+    <workbookView xWindow="5440" yWindow="500" windowWidth="28980" windowHeight="21900" xr2:uid="{81031926-05D2-A343-B9B8-A8769874A27F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -10313,15 +10313,15 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.1640625" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="5" max="5" width="41.83203125" customWidth="1"/>
-    <col min="6" max="6" width="43.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="6" max="6" width="41.83203125" customWidth="1"/>
+    <col min="7" max="7" width="43.33203125" customWidth="1"/>
     <col min="8" max="8" width="107.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10330,22 +10330,22 @@
         <v>79</v>
       </c>
       <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>68</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>78</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
@@ -10380,22 +10380,22 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>1995</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
       </c>
       <c r="H2" t="s">
         <v>15</v>
@@ -10427,22 +10427,22 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
         <v>22</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>1995</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
       </c>
       <c r="H3" t="s">
         <v>29</v>
@@ -10472,22 +10472,22 @@
         <v>33</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>1995</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>32</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>69</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
       </c>
       <c r="H4" t="s">
         <v>34</v>
@@ -10514,22 +10514,22 @@
         <v>37</v>
       </c>
       <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>1995</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>36</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>38</v>
-      </c>
-      <c r="G5" t="s">
-        <v>40</v>
       </c>
       <c r="H5" t="s">
         <v>41</v>
@@ -10556,22 +10556,22 @@
         <v>43</v>
       </c>
       <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>1995</v>
-      </c>
-      <c r="D6" t="s">
-        <v>43</v>
       </c>
       <c r="E6" t="s">
         <v>43</v>
       </c>
       <c r="F6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" t="s">
         <v>44</v>
-      </c>
-      <c r="G6" t="s">
-        <v>45</v>
       </c>
       <c r="H6" t="s">
         <v>46</v>
@@ -10601,22 +10601,22 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>1995</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>50</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>51</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
@@ -10639,22 +10639,22 @@
         <v>33</v>
       </c>
       <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>1997</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>52</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>53</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>69</v>
-      </c>
-      <c r="G8" t="s">
-        <v>14</v>
       </c>
       <c r="H8" t="s">
         <v>75</v>
@@ -10677,22 +10677,22 @@
         <v>55</v>
       </c>
       <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>1998</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>52</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>54</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>74</v>
-      </c>
-      <c r="G9" t="s">
-        <v>56</v>
       </c>
       <c r="H9" t="s">
         <v>73</v>
@@ -10712,22 +10712,22 @@
         <v>60</v>
       </c>
       <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
         <v>57</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>2001</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>58</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>59</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>70</v>
-      </c>
-      <c r="G10" t="s">
-        <v>40</v>
       </c>
       <c r="H10" t="s">
         <v>71</v>
@@ -10750,22 +10750,22 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
         <v>62</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>2013</v>
-      </c>
-      <c r="D11" t="s">
-        <v>63</v>
       </c>
       <c r="E11" t="s">
         <v>63</v>
       </c>
       <c r="F11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" t="s">
         <v>26</v>
-      </c>
-      <c r="G11" t="s">
-        <v>28</v>
       </c>
       <c r="H11" t="s">
         <v>29</v>
@@ -10795,22 +10795,22 @@
         <v>65</v>
       </c>
       <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
         <v>62</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>2013</v>
-      </c>
-      <c r="D12" t="s">
-        <v>65</v>
       </c>
       <c r="E12" t="s">
         <v>65</v>
       </c>
       <c r="F12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" t="s">
         <v>66</v>
-      </c>
-      <c r="G12" t="s">
-        <v>40</v>
       </c>
       <c r="H12" t="s">
         <v>77</v>

</xml_diff>